<commit_message>
Fixed some bugs, AI bets and plays correctly
</commit_message>
<xml_diff>
--- a/CST407FinalBlackJack/Resources/Blackjack Betting System.xlsx
+++ b/CST407FinalBlackJack/Resources/Blackjack Betting System.xlsx
@@ -31,10 +31,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -93,13 +93,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -470,7 +470,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1"/>
@@ -524,7 +524,7 @@
     </row>
     <row r="2" customHeight="1" spans="1:26">
       <c r="A2" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -579,22 +579,22 @@
     </row>
     <row r="3" customHeight="1" spans="1:25">
       <c r="A3" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>1</v>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>0</v>
@@ -634,31 +634,31 @@
     </row>
     <row r="4" customHeight="1" spans="1:25">
       <c r="A4" s="1">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>0</v>
@@ -689,43 +689,43 @@
     </row>
     <row r="5" customHeight="1" spans="1:25">
       <c r="A5" s="1">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>0</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="6" customHeight="1" spans="1:25">
       <c r="A6" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>0</v>
@@ -752,14 +752,14 @@
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
+      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>0</v>
@@ -799,22 +799,22 @@
     </row>
     <row r="7" customHeight="1" spans="1:25">
       <c r="A7" s="1">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>0</v>
@@ -854,22 +854,22 @@
     </row>
     <row r="8" customHeight="1" spans="1:25">
       <c r="A8" s="1">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>0</v>
@@ -909,22 +909,22 @@
     </row>
     <row r="9" customHeight="1" spans="1:25">
       <c r="A9" s="1">
-        <v>15</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>0</v>
@@ -964,31 +964,31 @@
     </row>
     <row r="10" customHeight="1" spans="1:25">
       <c r="A10" s="1">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>0</v>
@@ -1019,46 +1019,46 @@
     </row>
     <row r="11" customHeight="1" spans="1:25">
       <c r="A11" s="1">
-        <v>17</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
@@ -1073,14 +1073,14 @@
       <c r="Y11" s="5"/>
     </row>
     <row r="12" customHeight="1" spans="1:25">
-      <c r="A12" s="4">
-        <v>18</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
+      <c r="A12" s="1">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>2</v>
@@ -1091,29 +1091,29 @@
       <c r="F12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>2</v>
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
@@ -1128,8 +1128,8 @@
       <c r="Y12" s="5"/>
     </row>
     <row r="13" customHeight="1" spans="1:25">
-      <c r="A13" s="4">
-        <v>19</v>
+      <c r="A13" s="1">
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>2</v>
@@ -1146,29 +1146,29 @@
       <c r="F13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>2</v>
+      <c r="G13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
@@ -1183,8 +1183,8 @@
       <c r="Y13" s="5"/>
     </row>
     <row r="14" customHeight="1" spans="1:25">
-      <c r="A14" s="4">
-        <v>20</v>
+      <c r="A14" s="1">
+        <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>2</v>
@@ -1201,29 +1201,29 @@
       <c r="F14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>2</v>
+      <c r="G14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
@@ -1238,8 +1238,8 @@
       <c r="Y14" s="5"/>
     </row>
     <row r="15" customHeight="1" spans="1:25">
-      <c r="A15" s="4">
-        <v>21</v>
+      <c r="A15" s="1">
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>2</v>
@@ -1256,29 +1256,29 @@
       <c r="F15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>2</v>
+      <c r="G15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
@@ -1294,22 +1294,22 @@
     </row>
     <row r="16" customHeight="1" spans="1:25">
       <c r="A16" s="1">
-        <v>142</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>0</v>
@@ -1349,46 +1349,46 @@
     </row>
     <row r="17" customHeight="1" spans="1:25">
       <c r="A17" s="1">
-        <v>143</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
@@ -1403,47 +1403,47 @@
       <c r="Y17" s="5"/>
     </row>
     <row r="18" customHeight="1" spans="1:25">
-      <c r="A18" s="1">
-        <v>144</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>0</v>
+      <c r="A18" s="4">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
@@ -1458,47 +1458,47 @@
       <c r="Y18" s="5"/>
     </row>
     <row r="19" customHeight="1" spans="1:25">
-      <c r="A19" s="1">
-        <v>145</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>0</v>
+      <c r="A19" s="4">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
@@ -1513,47 +1513,47 @@
       <c r="Y19" s="5"/>
     </row>
     <row r="20" customHeight="1" spans="1:26">
-      <c r="A20" s="1">
-        <v>146</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>0</v>
+      <c r="A20" s="4">
+        <v>20</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
@@ -1569,23 +1569,23 @@
       <c r="Z20" s="5"/>
     </row>
     <row r="21" customHeight="1" spans="1:26">
-      <c r="A21" s="1">
-        <v>147</v>
+      <c r="A21" s="4">
+        <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>1</v>
+      <c r="C21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>2</v>
@@ -1593,23 +1593,23 @@
       <c r="H21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>0</v>
+      <c r="I21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
@@ -1626,46 +1626,46 @@
     </row>
     <row r="22" customHeight="1" spans="1:26">
       <c r="A22" s="1">
-        <v>148</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>2</v>
+        <v>142</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
@@ -1681,20 +1681,48 @@
       <c r="Z22" s="5"/>
     </row>
     <row r="23" customHeight="1" spans="1:26">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
+      <c r="A23" s="1">
+        <v>143</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
@@ -1709,20 +1737,48 @@
       <c r="Z23" s="5"/>
     </row>
     <row r="24" customHeight="1" spans="1:26">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
+      <c r="A24" s="1">
+        <v>144</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
@@ -1737,20 +1793,48 @@
       <c r="Z24" s="5"/>
     </row>
     <row r="25" customHeight="1" spans="1:26">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
+      <c r="A25" s="1">
+        <v>145</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
@@ -1765,20 +1849,48 @@
       <c r="Z25" s="5"/>
     </row>
     <row r="26" customHeight="1" spans="1:26">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
+      <c r="A26" s="1">
+        <v>146</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
@@ -1793,20 +1905,48 @@
       <c r="Z26" s="5"/>
     </row>
     <row r="27" customHeight="1" spans="1:26">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
+      <c r="A27" s="1">
+        <v>147</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
@@ -1821,20 +1961,48 @@
       <c r="Z27" s="5"/>
     </row>
     <row r="28" customHeight="1" spans="1:26">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
+      <c r="A28" s="1">
+        <v>148</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
@@ -28952,18 +29120,7 @@
       <c r="Y996" s="5"/>
       <c r="Z996" s="5"/>
     </row>
-    <row r="997" customHeight="1" spans="1:26">
-      <c r="A997" s="5"/>
-      <c r="B997" s="5"/>
-      <c r="C997" s="5"/>
-      <c r="D997" s="5"/>
-      <c r="E997" s="5"/>
-      <c r="F997" s="5"/>
-      <c r="G997" s="5"/>
-      <c r="H997" s="5"/>
-      <c r="I997" s="5"/>
-      <c r="J997" s="5"/>
-      <c r="K997" s="5"/>
+    <row r="997" customHeight="1" spans="12:26">
       <c r="L997" s="5"/>
       <c r="M997" s="5"/>
       <c r="N997" s="5"/>
@@ -28980,21 +29137,7 @@
       <c r="Y997" s="5"/>
       <c r="Z997" s="5"/>
     </row>
-    <row r="998" customHeight="1" spans="1:26">
-      <c r="A998" s="5"/>
-      <c r="B998" s="5"/>
-      <c r="C998" s="5"/>
-      <c r="D998" s="5"/>
-      <c r="E998" s="5"/>
-      <c r="F998" s="5"/>
-      <c r="G998" s="5"/>
-      <c r="H998" s="5"/>
-      <c r="I998" s="5"/>
-      <c r="J998" s="5"/>
-      <c r="K998" s="5"/>
-      <c r="L998" s="5"/>
-      <c r="M998" s="5"/>
-      <c r="N998" s="5"/>
+    <row r="998" customHeight="1" spans="15:26">
       <c r="O998" s="5"/>
       <c r="P998" s="5"/>
       <c r="Q998" s="5"/>
@@ -29008,21 +29151,7 @@
       <c r="Y998" s="5"/>
       <c r="Z998" s="5"/>
     </row>
-    <row r="999" customHeight="1" spans="1:26">
-      <c r="A999" s="5"/>
-      <c r="B999" s="5"/>
-      <c r="C999" s="5"/>
-      <c r="D999" s="5"/>
-      <c r="E999" s="5"/>
-      <c r="F999" s="5"/>
-      <c r="G999" s="5"/>
-      <c r="H999" s="5"/>
-      <c r="I999" s="5"/>
-      <c r="J999" s="5"/>
-      <c r="K999" s="5"/>
-      <c r="L999" s="5"/>
-      <c r="M999" s="5"/>
-      <c r="N999" s="5"/>
+    <row r="999" customHeight="1" spans="15:26">
       <c r="O999" s="5"/>
       <c r="P999" s="5"/>
       <c r="Q999" s="5"/>
@@ -29036,10 +29165,7 @@
       <c r="Y999" s="5"/>
       <c r="Z999" s="5"/>
     </row>
-    <row r="1000" customHeight="1" spans="12:26">
-      <c r="L1000" s="5"/>
-      <c r="M1000" s="5"/>
-      <c r="N1000" s="5"/>
+    <row r="1000" customHeight="1" spans="15:26">
       <c r="O1000" s="5"/>
       <c r="P1000" s="5"/>
       <c r="Q1000" s="5"/>

</xml_diff>